<commit_message>
fix: header in dataset-evaluation-results.xlsx
Update manifest files to capture change. Fix to dataset_description
</commit_message>
<xml_diff>
--- a/dataset_description.xlsx
+++ b/dataset_description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BPatel\Documents\GitHub\FAIR-AMD-OCT-paper-dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D2E5F7-8BDD-486F-8F74-003DD348F875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF12495-73A8-46D8-8364-103D7D529B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
   <si>
     <t>Metadata element</t>
   </si>
@@ -239,9 +239,6 @@
   </si>
   <si>
     <t>spinal cord</t>
-  </si>
-  <si>
-    <t>autonomic ganglion</t>
   </si>
   <si>
     <t xml:space="preserve">    Study approach</t>
@@ -1083,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1364,56 +1361,54 @@
       <c r="C14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D14" t="s">
-        <v>54</v>
-      </c>
+      <c r="D14"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>59</v>
-      </c>
-      <c r="F15" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="C16" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" t="s">
         <v>63</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>64</v>
-      </c>
-      <c r="E16" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="C17" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="D17"/>
       <c r="E17" s="29"/>
@@ -1425,7 +1420,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="14"/>
       <c r="C18" s="15"/>
@@ -1439,132 +1434,132 @@
     </row>
     <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="C19" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>74</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>75</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>76</v>
       </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>77</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>78</v>
-      </c>
-      <c r="J19" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="23" t="str">
         <f>HYPERLINK("https://orcid.org/","ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.")</f>
         <v>ORCiD ID. If you don't have an ORCiD, we suggest you sign up for one.</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" t="s">
         <v>82</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>83</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>84</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>85</v>
-      </c>
-      <c r="J20" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="C21" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="D21" t="s">
         <v>89</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>89</v>
+      </c>
+      <c r="G21" t="s">
         <v>90</v>
       </c>
-      <c r="E21" t="s">
+      <c r="H21" t="s">
         <v>90</v>
       </c>
-      <c r="F21" t="s">
+      <c r="I21" t="s">
         <v>90</v>
       </c>
-      <c r="G21" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" t="s">
-        <v>91</v>
-      </c>
-      <c r="I21" t="s">
-        <v>91</v>
-      </c>
       <c r="J21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="C22" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D22" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" t="s">
+        <v>94</v>
+      </c>
+      <c r="G22" t="s">
+        <v>93</v>
+      </c>
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" t="s">
         <v>95</v>
       </c>
-      <c r="E22" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" t="s">
-        <v>95</v>
-      </c>
-      <c r="G22" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" t="s">
-        <v>94</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>96</v>
-      </c>
-      <c r="J22" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
@@ -1578,64 +1573,64 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="C24" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="D24" s="24" t="s">
         <v>101</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>102</v>
       </c>
       <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="C25" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="D25" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="C26" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="D26" t="s">
         <v>109</v>
-      </c>
-      <c r="D26" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="C27" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="D27" t="s">
         <v>113</v>
-      </c>
-      <c r="D27" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -1649,10 +1644,10 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>117</v>
       </c>
       <c r="C29" s="12">
         <v>1</v>
@@ -1669,10 +1664,10 @@
     </row>
     <row r="30" spans="1:10" ht="15.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>118</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>119</v>
       </c>
       <c r="C30" s="12">
         <v>0</v>

</xml_diff>